<commit_message>
Estilização de Excel de dividas de ISS.
</commit_message>
<xml_diff>
--- a/PrototipoAnapolis/Dividas Diversas.xlsx
+++ b/PrototipoAnapolis/Dividas Diversas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="46">
   <si>
     <t>Inscrição</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>53073</t>
+  </si>
+  <si>
+    <t>Totais R$:</t>
   </si>
   <si>
     <t>Inscrição ISS</t>
@@ -155,7 +158,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,8 +174,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,6 +199,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6E2FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF666666"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -219,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -228,6 +245,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -524,7 +544,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N117"/>
+  <dimension ref="A1:N118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -584,19 +604,19 @@
         <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I3" s="3">
         <v>250.93</v>
@@ -622,19 +642,19 @@
         <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I4" s="2">
         <v>67.2</v>
@@ -660,19 +680,19 @@
         <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I5" s="3">
         <v>9.81</v>
@@ -698,19 +718,19 @@
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I6" s="2">
         <v>26.86</v>
@@ -736,19 +756,19 @@
         <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I7" s="3">
         <v>1.65</v>
@@ -774,19 +794,19 @@
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I8" s="2">
         <v>190.95</v>
@@ -812,19 +832,19 @@
         <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I9" s="3">
         <v>184.96</v>
@@ -850,19 +870,19 @@
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I10" s="2">
         <v>218.75</v>
@@ -888,19 +908,19 @@
         <v>15</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I11" s="3">
         <v>24.17</v>
@@ -926,19 +946,19 @@
         <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I12" s="2">
         <v>5.22</v>
@@ -964,19 +984,19 @@
         <v>15</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I13" s="3">
         <v>5.22</v>
@@ -1002,19 +1022,19 @@
         <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I14" s="2">
         <v>15150.35</v>
@@ -1040,19 +1060,19 @@
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I15" s="3">
         <v>7249.8</v>
@@ -1078,19 +1098,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I16" s="2">
         <v>8890.290000000001</v>
@@ -1116,19 +1136,19 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I17" s="3">
         <v>300</v>
@@ -1154,19 +1174,19 @@
         <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I18" s="2">
         <v>375</v>
@@ -1192,19 +1212,19 @@
         <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I19" s="3">
         <v>5.2</v>
@@ -1230,19 +1250,19 @@
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I20" s="2">
         <v>7.7</v>
@@ -1268,19 +1288,19 @@
         <v>15</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I21" s="3">
         <v>118.1</v>
@@ -1306,19 +1326,19 @@
         <v>15</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I22" s="2">
         <v>76.48</v>
@@ -1344,19 +1364,19 @@
         <v>15</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I23" s="3">
         <v>332.06</v>
@@ -1382,19 +1402,19 @@
         <v>15</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I24" s="2">
         <v>24.51</v>
@@ -1420,19 +1440,19 @@
         <v>15</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I25" s="3">
         <v>804</v>
@@ -1458,19 +1478,19 @@
         <v>15</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I26" s="2">
         <v>38.56</v>
@@ -1496,19 +1516,19 @@
         <v>15</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I27" s="3">
         <v>85.03</v>
@@ -1534,19 +1554,19 @@
         <v>15</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I28" s="2">
         <v>218.75</v>
@@ -1572,19 +1592,19 @@
         <v>15</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I29" s="3">
         <v>1161.22</v>
@@ -1610,19 +1630,19 @@
         <v>15</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I30" s="2">
         <v>844.8</v>
@@ -1648,19 +1668,19 @@
         <v>15</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I31" s="3">
         <v>3050.86</v>
@@ -1686,19 +1706,19 @@
         <v>15</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I32" s="2">
         <v>408.5</v>
@@ -1724,19 +1744,19 @@
         <v>15</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I33" s="3">
         <v>408.5</v>
@@ -1762,19 +1782,19 @@
         <v>15</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I34" s="2">
         <v>218.75</v>
@@ -1800,19 +1820,19 @@
         <v>15</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I35" s="3">
         <v>218.75</v>
@@ -1838,19 +1858,19 @@
         <v>15</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I36" s="2">
         <v>179.6</v>
@@ -1876,19 +1896,19 @@
         <v>15</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I37" s="3">
         <v>60</v>
@@ -1914,19 +1934,19 @@
         <v>15</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I38" s="2">
         <v>19.46</v>
@@ -1952,19 +1972,19 @@
         <v>15</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I39" s="3">
         <v>5665.73</v>
@@ -1990,19 +2010,19 @@
         <v>15</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I40" s="2">
         <v>71.83</v>
@@ -2028,19 +2048,19 @@
         <v>15</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I41" s="3">
         <v>1175</v>
@@ -2066,19 +2086,19 @@
         <v>15</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I42" s="2">
         <v>179.85</v>
@@ -2104,19 +2124,19 @@
         <v>15</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I43" s="3">
         <v>4.5</v>
@@ -2142,19 +2162,19 @@
         <v>15</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I44" s="2">
         <v>562.0700000000001</v>
@@ -2180,19 +2200,19 @@
         <v>15</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I45" s="3">
         <v>100</v>
@@ -2218,19 +2238,19 @@
         <v>15</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I46" s="2">
         <v>150</v>
@@ -2256,19 +2276,19 @@
         <v>15</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I47" s="3">
         <v>147.84</v>
@@ -2294,19 +2314,19 @@
         <v>15</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I48" s="2">
         <v>9</v>
@@ -2332,19 +2352,19 @@
         <v>15</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I49" s="3">
         <v>187.5</v>
@@ -2370,19 +2390,19 @@
         <v>15</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I50" s="2">
         <v>192.1</v>
@@ -2408,19 +2428,19 @@
         <v>15</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I51" s="3">
         <v>187.5</v>
@@ -2446,19 +2466,19 @@
         <v>15</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I52" s="2">
         <v>5.22</v>
@@ -2484,19 +2504,19 @@
         <v>15</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I53" s="3">
         <v>40.45</v>
@@ -2522,19 +2542,19 @@
         <v>15</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I54" s="2">
         <v>5.22</v>
@@ -2560,19 +2580,19 @@
         <v>15</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I55" s="3">
         <v>13.4</v>
@@ -2598,19 +2618,19 @@
         <v>15</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I56" s="2">
         <v>100</v>
@@ -2636,19 +2656,19 @@
         <v>15</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I57" s="3">
         <v>24.17</v>
@@ -2674,19 +2694,19 @@
         <v>15</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I58" s="2">
         <v>260.06</v>
@@ -2712,19 +2732,19 @@
         <v>15</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I59" s="3">
         <v>260.06</v>
@@ -2750,19 +2770,19 @@
         <v>15</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I60" s="2">
         <v>17.24</v>
@@ -2788,19 +2808,19 @@
         <v>15</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I61" s="3">
         <v>70.94</v>
@@ -2826,19 +2846,19 @@
         <v>15</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I62" s="2">
         <v>28.88</v>
@@ -2864,19 +2884,19 @@
         <v>15</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I63" s="3">
         <v>5000</v>
@@ -2902,19 +2922,19 @@
         <v>15</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I64" s="2">
         <v>5000</v>
@@ -2940,19 +2960,19 @@
         <v>15</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I65" s="3">
         <v>12.37</v>
@@ -2978,19 +2998,19 @@
         <v>15</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I66" s="2">
         <v>5.56</v>
@@ -3016,19 +3036,19 @@
         <v>15</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I67" s="3">
         <v>30.39</v>
@@ -3054,19 +3074,19 @@
         <v>15</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I68" s="2">
         <v>292.76</v>
@@ -3092,19 +3112,19 @@
         <v>15</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I69" s="3">
         <v>0.71</v>
@@ -3130,19 +3150,19 @@
         <v>15</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I70" s="2">
         <v>1.22</v>
@@ -3168,19 +3188,19 @@
         <v>15</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I71" s="3">
         <v>0.71</v>
@@ -3206,19 +3226,19 @@
         <v>15</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I72" s="2">
         <v>38.84</v>
@@ -3244,19 +3264,19 @@
         <v>15</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I73" s="3">
         <v>25.53</v>
@@ -3282,19 +3302,19 @@
         <v>15</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I74" s="2">
         <v>128.27</v>
@@ -3320,19 +3340,19 @@
         <v>15</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I75" s="3">
         <v>25.53</v>
@@ -3358,19 +3378,19 @@
         <v>15</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I76" s="2">
         <v>7.66</v>
@@ -3396,19 +3416,19 @@
         <v>15</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I77" s="3">
         <v>95</v>
@@ -3434,19 +3454,19 @@
         <v>15</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I78" s="2">
         <v>101.39</v>
@@ -3472,19 +3492,19 @@
         <v>15</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I79" s="3">
         <v>7.84</v>
@@ -3510,19 +3530,19 @@
         <v>15</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I80" s="2">
         <v>140.91</v>
@@ -3548,19 +3568,19 @@
         <v>15</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I81" s="3">
         <v>27.33</v>
@@ -3586,19 +3606,19 @@
         <v>15</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I82" s="2">
         <v>61.23</v>
@@ -3624,19 +3644,19 @@
         <v>15</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I83" s="3">
         <v>61.72</v>
@@ -3662,19 +3682,19 @@
         <v>15</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I84" s="2">
         <v>2307.99</v>
@@ -3700,19 +3720,19 @@
         <v>15</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I85" s="3">
         <v>3097.53</v>
@@ -3738,19 +3758,19 @@
         <v>15</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I86" s="2">
         <v>229.28</v>
@@ -3776,19 +3796,19 @@
         <v>15</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I87" s="3">
         <v>39.85</v>
@@ -3814,19 +3834,19 @@
         <v>15</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I88" s="2">
         <v>40.81</v>
@@ -3852,19 +3872,19 @@
         <v>15</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I89" s="3">
         <v>187.55</v>
@@ -3890,19 +3910,19 @@
         <v>15</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I90" s="2">
         <v>44.28</v>
@@ -3928,19 +3948,19 @@
         <v>15</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I91" s="3">
         <v>39.85</v>
@@ -3966,19 +3986,19 @@
         <v>15</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I92" s="2">
         <v>11.92</v>
@@ -4004,19 +4024,19 @@
         <v>15</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I93" s="3">
         <v>22.18</v>
@@ -4042,19 +4062,19 @@
         <v>15</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I94" s="2">
         <v>569.3099999999999</v>
@@ -4080,19 +4100,19 @@
         <v>15</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H95" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I95" s="3">
         <v>166.88</v>
@@ -4118,19 +4138,19 @@
         <v>15</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I96" s="2">
         <v>67.04000000000001</v>
@@ -4156,19 +4176,19 @@
         <v>15</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I97" s="3">
         <v>55.13</v>
@@ -4194,19 +4214,19 @@
         <v>15</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I98" s="2">
         <v>19.96</v>
@@ -4232,19 +4252,19 @@
         <v>15</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I99" s="3">
         <v>13.86</v>
@@ -4270,19 +4290,19 @@
         <v>15</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I100" s="2">
         <v>58.22</v>
@@ -4308,19 +4328,19 @@
         <v>15</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I101" s="3">
         <v>24.95</v>
@@ -4346,19 +4366,19 @@
         <v>15</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I102" s="2">
         <v>46.58</v>
@@ -4384,19 +4404,19 @@
         <v>15</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I103" s="3">
         <v>23.58</v>
@@ -4422,19 +4442,19 @@
         <v>15</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I104" s="2">
         <v>679.8200000000001</v>
@@ -4460,19 +4480,19 @@
         <v>15</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I105" s="3">
         <v>11.23</v>
@@ -4498,19 +4518,19 @@
         <v>15</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I106" s="2">
         <v>7.85</v>
@@ -4536,19 +4556,19 @@
         <v>15</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I107" s="3">
         <v>11.25</v>
@@ -4574,19 +4594,19 @@
         <v>15</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I108" s="2">
         <v>20.37</v>
@@ -4612,19 +4632,19 @@
         <v>15</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H109" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I109" s="3">
         <v>735.8</v>
@@ -4650,19 +4670,19 @@
         <v>15</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I110" s="2">
         <v>60</v>
@@ -4688,19 +4708,19 @@
         <v>15</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H111" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I111" s="3">
         <v>7.85</v>
@@ -4726,19 +4746,19 @@
         <v>15</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I112" s="2">
         <v>18.85</v>
@@ -4764,19 +4784,19 @@
         <v>15</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H113" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I113" s="3">
         <v>55.84</v>
@@ -4802,19 +4822,19 @@
         <v>15</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I114" s="2">
         <v>55.84</v>
@@ -4840,19 +4860,19 @@
         <v>15</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I115" s="3">
         <v>35.1</v>
@@ -4878,19 +4898,19 @@
         <v>15</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I116" s="2">
         <v>31.78</v>
@@ -4916,19 +4936,19 @@
         <v>15</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H117" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I117" s="3">
         <v>264.59</v>
@@ -4947,6 +4967,11 @@
       </c>
       <c r="N117" s="3">
         <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" s="4" customFormat="1">
+      <c r="A118" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refinamento de processamento de planilhas
</commit_message>
<xml_diff>
--- a/PrototipoAnapolis/Dividas Diversas.xlsx
+++ b/PrototipoAnapolis/Dividas Diversas.xlsx
@@ -549,6 +549,13 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
@@ -598,6 +605,18 @@
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
@@ -4972,6 +4991,18 @@
     <row r="118" spans="1:14" s="4" customFormat="1">
       <c r="A118" s="4" t="s">
         <v>16</v>
+      </c>
+      <c r="I118" s="4">
+        <v>70818.43999999999</v>
+      </c>
+      <c r="J118" s="4">
+        <v>3257.12</v>
+      </c>
+      <c r="K118" s="4">
+        <v>233.7499999999999</v>
+      </c>
+      <c r="L118" s="4">
+        <v>74309.30999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>